<commit_message>
encoding = 'UTF-8' added
</commit_message>
<xml_diff>
--- a/data/BFI.xlsx
+++ b/data/BFI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coop2711/Google 드라이브/Works/Class/Data_Science/R.WD/r_programming_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0095EC0-C311-874B-BA55-F64389C38E19}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D6D701-8397-1040-A2F9-4B5ACA727810}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53140" yWindow="3420" windowWidth="47300" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11980" yWindow="4860" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>학(직)번</t>
-  </si>
-  <si>
-    <t>E!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>A1</t>
@@ -78,6 +74,10 @@
   </si>
   <si>
     <t>A3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -547,7 +547,7 @@
   <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -571,40 +571,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">

</xml_diff>